<commit_message>
Creación de interfaz y modificación de plantilla de tareas
Se creo la inter gráfica de crear renta y se modifico la plantilla con tareas no previstas durante la planeación de la iteración presente
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 5/Plantilla Lista de Tareas de la Entrega 5.xlsx
+++ b/Plantillas/Entrega 5/Plantilla Lista de Tareas de la Entrega 5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8898BAFE-6039-4658-9DDC-15D5B7A6F870}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D86D5F1-22AB-43A5-A94D-A0D583DE0BA7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Instructivo" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Casos de Uso'!$A$1:$BB$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Casos de Uso'!$A$1:$BB$38</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="70">
   <si>
     <t>Columna</t>
   </si>
@@ -221,6 +221,27 @@
   </si>
   <si>
     <t>Hecho</t>
+  </si>
+  <si>
+    <t>CU-14</t>
+  </si>
+  <si>
+    <t>En este caso de uso el Director podrá dar de alta un nuevo Maestro en el sistema.</t>
+  </si>
+  <si>
+    <t>Correciones de implementación</t>
+  </si>
+  <si>
+    <t>CU-15</t>
+  </si>
+  <si>
+    <t>En este caso de uso el Director podrá modificar la información personal de un Maestro registrado en el sistema.</t>
+  </si>
+  <si>
+    <t>En proceso</t>
+  </si>
+  <si>
+    <t>Codificación</t>
   </si>
 </sst>
 </file>
@@ -871,13 +892,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:BB32"/>
+  <dimension ref="B1:BB37"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="M6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AD14" sqref="AD14"/>
+      <selection pane="bottomRight" activeCell="BA31" sqref="BA31:BA32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +906,7 @@
     <col min="1" max="1" width="3.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="54.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" style="16" customWidth="1"/>
@@ -1241,85 +1262,85 @@
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14">
-        <f t="shared" ref="I7:I31" si="0">G7-H7</f>
+        <f t="shared" ref="I7:I36" si="0">G7-H7</f>
         <v>2</v>
       </c>
       <c r="J7" s="15"/>
       <c r="K7" s="14"/>
       <c r="L7" s="14">
-        <f t="shared" ref="L7:L31" si="1">I7-K7</f>
+        <f t="shared" ref="L7:L36" si="1">I7-K7</f>
         <v>2</v>
       </c>
       <c r="M7" s="15"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14">
-        <f t="shared" ref="O7:O31" si="2">L7-N7</f>
+        <f t="shared" ref="O7:O36" si="2">L7-N7</f>
         <v>2</v>
       </c>
       <c r="P7" s="15"/>
       <c r="Q7" s="14"/>
       <c r="R7" s="14">
-        <f t="shared" ref="R7:R31" si="3">O7-Q7</f>
+        <f t="shared" ref="R7:R36" si="3">O7-Q7</f>
         <v>2</v>
       </c>
       <c r="S7" s="15"/>
       <c r="T7" s="14"/>
       <c r="U7" s="14">
-        <f t="shared" ref="U7:U31" si="4">R7-T7</f>
+        <f t="shared" ref="U7:U36" si="4">R7-T7</f>
         <v>2</v>
       </c>
       <c r="V7" s="14"/>
       <c r="W7" s="14"/>
       <c r="X7" s="14">
-        <f t="shared" ref="X7:X31" si="5">U7-W7</f>
+        <f t="shared" ref="X7:X36" si="5">U7-W7</f>
         <v>2</v>
       </c>
       <c r="Y7" s="14"/>
       <c r="Z7" s="14"/>
       <c r="AA7" s="14">
-        <f t="shared" ref="AA7:AA31" si="6">X7-Z7</f>
+        <f t="shared" ref="AA7:AA36" si="6">X7-Z7</f>
         <v>2</v>
       </c>
       <c r="AB7" s="14"/>
       <c r="AC7" s="14"/>
       <c r="AD7" s="14">
-        <f t="shared" ref="AD7:AD31" si="7">AA7-AC7</f>
+        <f t="shared" ref="AD7:AD36" si="7">AA7-AC7</f>
         <v>2</v>
       </c>
       <c r="AE7" s="14"/>
       <c r="AF7" s="14"/>
       <c r="AG7" s="14">
-        <f t="shared" ref="AG7:AG31" si="8">AD7-AF7</f>
+        <f t="shared" ref="AG7:AG36" si="8">AD7-AF7</f>
         <v>2</v>
       </c>
       <c r="AH7" s="14"/>
       <c r="AI7" s="14"/>
       <c r="AJ7" s="14">
-        <f t="shared" ref="AJ7:AJ31" si="9">AG7-AI7</f>
+        <f t="shared" ref="AJ7:AJ36" si="9">AG7-AI7</f>
         <v>2</v>
       </c>
       <c r="AK7" s="14"/>
       <c r="AL7" s="14"/>
       <c r="AM7" s="14">
-        <f t="shared" ref="AM7:AM31" si="10">AJ7-AL7</f>
+        <f t="shared" ref="AM7:AM36" si="10">AJ7-AL7</f>
         <v>2</v>
       </c>
       <c r="AN7" s="14"/>
       <c r="AO7" s="14"/>
       <c r="AP7" s="14">
-        <f t="shared" ref="AP7:AP31" si="11">AM7-AO7</f>
+        <f t="shared" ref="AP7:AP36" si="11">AM7-AO7</f>
         <v>2</v>
       </c>
       <c r="AQ7" s="14"/>
       <c r="AR7" s="14"/>
       <c r="AS7" s="14">
-        <f t="shared" ref="AS7:AS31" si="12">AP7-AR7</f>
+        <f t="shared" ref="AS7:AS36" si="12">AP7-AR7</f>
         <v>2</v>
       </c>
       <c r="AT7" s="14"/>
       <c r="AU7" s="14"/>
       <c r="AV7" s="14">
-        <f t="shared" ref="AV7:AV31" si="13">AS7-AU7</f>
+        <f t="shared" ref="AV7:AV36" si="13">AS7-AU7</f>
         <v>2</v>
       </c>
       <c r="AW7" s="14"/>
@@ -1501,7 +1522,7 @@
         <v>2</v>
       </c>
       <c r="AZ9" s="35">
-        <f t="shared" ref="AZ9:AZ31" si="14">H9+K9+N9+Q9+T9+W9+Z9+AC9+AF9+AI9+AL9+AO9+AR9+AU9+AX9</f>
+        <f t="shared" ref="AZ9:AZ36" si="14">H9+K9+N9+Q9+T9+W9+Z9+AC9+AF9+AI9+AL9+AO9+AR9+AU9+AX9</f>
         <v>0</v>
       </c>
       <c r="BA9" s="35">
@@ -1611,7 +1632,7 @@
       <c r="AW10" s="22"/>
       <c r="AX10" s="22"/>
       <c r="AY10" s="22">
-        <f t="shared" ref="AY10:AY31" si="15">AV10-AX10</f>
+        <f t="shared" ref="AY10:AY36" si="15">AV10-AX10</f>
         <v>2</v>
       </c>
       <c r="AZ10" s="35">
@@ -3015,7 +3036,7 @@
         <v>42</v>
       </c>
       <c r="F25" s="42" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="G25" s="43">
         <v>2</v>
@@ -3056,66 +3077,68 @@
         <v>2</v>
       </c>
       <c r="Y25" s="39"/>
-      <c r="Z25" s="39"/>
+      <c r="Z25" s="39">
+        <v>1</v>
+      </c>
       <c r="AA25" s="39">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB25" s="39"/>
       <c r="AC25" s="39"/>
       <c r="AD25" s="39">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE25" s="39"/>
       <c r="AF25" s="39"/>
       <c r="AG25" s="39">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH25" s="39"/>
       <c r="AI25" s="39"/>
       <c r="AJ25" s="39">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK25" s="39"/>
       <c r="AL25" s="39"/>
       <c r="AM25" s="39">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN25" s="39"/>
       <c r="AO25" s="39"/>
       <c r="AP25" s="39">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ25" s="39"/>
       <c r="AR25" s="39"/>
       <c r="AS25" s="39">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT25" s="39"/>
       <c r="AU25" s="39"/>
       <c r="AV25" s="39">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW25" s="39"/>
       <c r="AX25" s="39"/>
       <c r="AY25" s="39">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ25" s="35">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA25" s="35">
         <f>G25-AZ25</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB25" s="2"/>
     </row>
@@ -3129,7 +3152,7 @@
         <v>42</v>
       </c>
       <c r="F26" s="42" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="G26" s="43">
         <v>2</v>
@@ -3170,66 +3193,68 @@
         <v>2</v>
       </c>
       <c r="Y26" s="39"/>
-      <c r="Z26" s="39"/>
+      <c r="Z26" s="39">
+        <v>1</v>
+      </c>
       <c r="AA26" s="39">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB26" s="39"/>
       <c r="AC26" s="39"/>
       <c r="AD26" s="39">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE26" s="39"/>
       <c r="AF26" s="39"/>
       <c r="AG26" s="39">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH26" s="39"/>
       <c r="AI26" s="39"/>
       <c r="AJ26" s="39">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK26" s="39"/>
       <c r="AL26" s="39"/>
       <c r="AM26" s="39">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN26" s="39"/>
       <c r="AO26" s="39"/>
       <c r="AP26" s="39">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ26" s="39"/>
       <c r="AR26" s="39"/>
       <c r="AS26" s="39">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT26" s="39"/>
       <c r="AU26" s="39"/>
       <c r="AV26" s="39">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW26" s="39"/>
       <c r="AX26" s="39"/>
       <c r="AY26" s="39">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ26" s="35">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA26" s="35">
         <f>G26-AZ26</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB26" s="2"/>
     </row>
@@ -3243,7 +3268,7 @@
         <v>42</v>
       </c>
       <c r="F27" s="42" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G27" s="43">
         <v>2</v>
@@ -3284,66 +3309,68 @@
         <v>2</v>
       </c>
       <c r="Y27" s="39"/>
-      <c r="Z27" s="39"/>
+      <c r="Z27" s="39">
+        <v>2</v>
+      </c>
       <c r="AA27" s="39">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB27" s="39"/>
       <c r="AC27" s="39"/>
       <c r="AD27" s="39">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE27" s="39"/>
       <c r="AF27" s="39"/>
       <c r="AG27" s="39">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH27" s="39"/>
       <c r="AI27" s="39"/>
       <c r="AJ27" s="39">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK27" s="39"/>
       <c r="AL27" s="39"/>
       <c r="AM27" s="39">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN27" s="39"/>
       <c r="AO27" s="39"/>
       <c r="AP27" s="39">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ27" s="39"/>
       <c r="AR27" s="39"/>
       <c r="AS27" s="39">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT27" s="39"/>
       <c r="AU27" s="39"/>
       <c r="AV27" s="39">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW27" s="39"/>
       <c r="AX27" s="39"/>
       <c r="AY27" s="39">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ27" s="35">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA27" s="35">
         <f>G27-AZ27</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BB27" s="2"/>
     </row>
@@ -3416,7 +3443,7 @@
         <v>42</v>
       </c>
       <c r="F29" s="39" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="G29" s="43">
         <v>2</v>
@@ -3451,72 +3478,74 @@
         <v>2</v>
       </c>
       <c r="V29" s="39"/>
-      <c r="W29" s="39"/>
+      <c r="W29" s="39">
+        <v>1</v>
+      </c>
       <c r="X29" s="39">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y29" s="39"/>
       <c r="Z29" s="39"/>
       <c r="AA29" s="39">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB29" s="39"/>
       <c r="AC29" s="39"/>
       <c r="AD29" s="39">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE29" s="39"/>
       <c r="AF29" s="39"/>
       <c r="AG29" s="39">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH29" s="39"/>
       <c r="AI29" s="39"/>
       <c r="AJ29" s="39">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK29" s="39"/>
       <c r="AL29" s="39"/>
       <c r="AM29" s="39">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN29" s="39"/>
       <c r="AO29" s="39"/>
       <c r="AP29" s="39">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ29" s="39"/>
       <c r="AR29" s="39"/>
       <c r="AS29" s="39">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT29" s="39"/>
       <c r="AU29" s="39"/>
       <c r="AV29" s="39">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW29" s="39"/>
       <c r="AX29" s="39"/>
       <c r="AY29" s="39">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ29" s="35">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA29" s="35">
         <f>G29-AZ29</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB29" s="2"/>
     </row>
@@ -3530,7 +3559,7 @@
         <v>42</v>
       </c>
       <c r="F30" s="39" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="G30" s="43">
         <v>2</v>
@@ -3565,72 +3594,74 @@
         <v>2</v>
       </c>
       <c r="V30" s="39"/>
-      <c r="W30" s="39"/>
+      <c r="W30" s="39">
+        <v>1</v>
+      </c>
       <c r="X30" s="39">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y30" s="39"/>
       <c r="Z30" s="39"/>
       <c r="AA30" s="39">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB30" s="39"/>
       <c r="AC30" s="39"/>
       <c r="AD30" s="39">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE30" s="39"/>
       <c r="AF30" s="39"/>
       <c r="AG30" s="39">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH30" s="39"/>
       <c r="AI30" s="39"/>
       <c r="AJ30" s="39">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK30" s="39"/>
       <c r="AL30" s="39"/>
       <c r="AM30" s="39">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN30" s="39"/>
       <c r="AO30" s="39"/>
       <c r="AP30" s="39">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ30" s="39"/>
       <c r="AR30" s="39"/>
       <c r="AS30" s="39">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT30" s="39"/>
       <c r="AU30" s="39"/>
       <c r="AV30" s="39">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW30" s="39"/>
       <c r="AX30" s="39"/>
       <c r="AY30" s="39">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ30" s="35">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA30" s="35">
         <f>G30-AZ30</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB30" s="2"/>
     </row>
@@ -3644,7 +3675,7 @@
         <v>42</v>
       </c>
       <c r="F31" s="39" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="G31" s="43">
         <v>2</v>
@@ -3691,124 +3722,585 @@
         <v>2</v>
       </c>
       <c r="AB31" s="39"/>
-      <c r="AC31" s="39"/>
+      <c r="AC31" s="39">
+        <v>1</v>
+      </c>
       <c r="AD31" s="39">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE31" s="39"/>
       <c r="AF31" s="39"/>
       <c r="AG31" s="39">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH31" s="39"/>
       <c r="AI31" s="39"/>
       <c r="AJ31" s="39">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK31" s="39"/>
       <c r="AL31" s="39"/>
       <c r="AM31" s="39">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN31" s="39"/>
       <c r="AO31" s="39"/>
       <c r="AP31" s="39">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ31" s="39"/>
       <c r="AR31" s="39"/>
       <c r="AS31" s="39">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT31" s="39"/>
       <c r="AU31" s="39"/>
       <c r="AV31" s="39">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW31" s="39"/>
       <c r="AX31" s="39"/>
       <c r="AY31" s="39">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ31" s="35">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA31" s="35">
         <f>G31-AZ31</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB31" s="2"/>
     </row>
-    <row r="32" spans="2:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="45"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="15"/>
-      <c r="T32" s="14"/>
-      <c r="U32" s="14"/>
-      <c r="V32" s="15"/>
-      <c r="W32" s="14"/>
-      <c r="X32" s="14"/>
-      <c r="Y32" s="15"/>
-      <c r="Z32" s="14"/>
-      <c r="AA32" s="14"/>
-      <c r="AB32" s="15"/>
-      <c r="AC32" s="14"/>
-      <c r="AD32" s="14"/>
-      <c r="AE32" s="15"/>
-      <c r="AF32" s="14"/>
-      <c r="AG32" s="14"/>
-      <c r="AH32" s="15"/>
-      <c r="AI32" s="14"/>
-      <c r="AJ32" s="14"/>
-      <c r="AK32" s="15"/>
-      <c r="AL32" s="14"/>
-      <c r="AM32" s="14"/>
-      <c r="AN32" s="15"/>
-      <c r="AO32" s="14"/>
-      <c r="AP32" s="14"/>
-      <c r="AQ32" s="15"/>
-      <c r="AR32" s="14"/>
-      <c r="AS32" s="14"/>
-      <c r="AT32" s="15"/>
-      <c r="AU32" s="14"/>
-      <c r="AV32" s="14"/>
-      <c r="AW32" s="15"/>
-      <c r="AX32" s="14"/>
-      <c r="AY32" s="14"/>
-      <c r="AZ32" s="14"/>
-      <c r="BA32" s="14"/>
+    <row r="32" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="42"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="43">
+        <v>4</v>
+      </c>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M32" s="39"/>
+      <c r="N32" s="39"/>
+      <c r="O32" s="39">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="P32" s="39"/>
+      <c r="Q32" s="39"/>
+      <c r="R32" s="39">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="S32" s="39"/>
+      <c r="T32" s="39"/>
+      <c r="U32" s="39">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="V32" s="39"/>
+      <c r="W32" s="39"/>
+      <c r="X32" s="39">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="Y32" s="39"/>
+      <c r="Z32" s="39"/>
+      <c r="AA32" s="39">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AB32" s="39"/>
+      <c r="AC32" s="39"/>
+      <c r="AD32" s="39">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="AE32" s="39"/>
+      <c r="AF32" s="39"/>
+      <c r="AG32" s="39">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AH32" s="39"/>
+      <c r="AI32" s="39"/>
+      <c r="AJ32" s="39">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="AK32" s="39"/>
+      <c r="AL32" s="39"/>
+      <c r="AM32" s="39">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="AN32" s="39"/>
+      <c r="AO32" s="39"/>
+      <c r="AP32" s="39">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="AQ32" s="39"/>
+      <c r="AR32" s="39"/>
+      <c r="AS32" s="39">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="AT32" s="39"/>
+      <c r="AU32" s="39"/>
+      <c r="AV32" s="39">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="AW32" s="39"/>
+      <c r="AX32" s="39"/>
+      <c r="AY32" s="39">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+      <c r="AZ32" s="35">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="BA32" s="35">
+        <f>G32-AZ32</f>
+        <v>4</v>
+      </c>
+      <c r="BB32" s="2"/>
+    </row>
+    <row r="33" spans="2:54" s="41" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="39"/>
+      <c r="O33" s="39"/>
+      <c r="P33" s="39"/>
+      <c r="Q33" s="39"/>
+      <c r="R33" s="39"/>
+      <c r="S33" s="39"/>
+      <c r="T33" s="39"/>
+      <c r="U33" s="39"/>
+      <c r="V33" s="39"/>
+      <c r="W33" s="39"/>
+      <c r="X33" s="39"/>
+      <c r="Y33" s="39"/>
+      <c r="Z33" s="39"/>
+      <c r="AA33" s="39"/>
+      <c r="AB33" s="39"/>
+      <c r="AC33" s="39"/>
+      <c r="AD33" s="39"/>
+      <c r="AE33" s="39"/>
+      <c r="AF33" s="39"/>
+      <c r="AG33" s="39"/>
+      <c r="AH33" s="39"/>
+      <c r="AI33" s="39"/>
+      <c r="AJ33" s="39"/>
+      <c r="AK33" s="39"/>
+      <c r="AL33" s="39"/>
+      <c r="AM33" s="39"/>
+      <c r="AN33" s="39"/>
+      <c r="AO33" s="39"/>
+      <c r="AP33" s="39"/>
+      <c r="AQ33" s="39"/>
+      <c r="AR33" s="39"/>
+      <c r="AS33" s="39"/>
+      <c r="AT33" s="39"/>
+      <c r="AU33" s="39"/>
+      <c r="AV33" s="39"/>
+      <c r="AW33" s="39"/>
+      <c r="AX33" s="39"/>
+      <c r="AY33" s="39"/>
+      <c r="AZ33" s="35"/>
+      <c r="BA33" s="35"/>
+      <c r="BB33" s="2"/>
+    </row>
+    <row r="34" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="42"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" s="43">
+        <v>2</v>
+      </c>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J34" s="39"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M34" s="39"/>
+      <c r="N34" s="39"/>
+      <c r="O34" s="39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P34" s="39"/>
+      <c r="Q34" s="39">
+        <v>2</v>
+      </c>
+      <c r="R34" s="39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S34" s="39"/>
+      <c r="T34" s="39"/>
+      <c r="U34" s="39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V34" s="39"/>
+      <c r="W34" s="39"/>
+      <c r="X34" s="39">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Y34" s="39"/>
+      <c r="Z34" s="39"/>
+      <c r="AA34" s="39">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AB34" s="39"/>
+      <c r="AC34" s="39"/>
+      <c r="AD34" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AE34" s="39"/>
+      <c r="AF34" s="39"/>
+      <c r="AG34" s="39">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AH34" s="39"/>
+      <c r="AI34" s="39"/>
+      <c r="AJ34" s="39">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AK34" s="39"/>
+      <c r="AL34" s="39"/>
+      <c r="AM34" s="39">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AN34" s="39"/>
+      <c r="AO34" s="39"/>
+      <c r="AP34" s="39">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AQ34" s="39"/>
+      <c r="AR34" s="39"/>
+      <c r="AS34" s="39">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AT34" s="39"/>
+      <c r="AU34" s="39"/>
+      <c r="AV34" s="39">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AW34" s="39"/>
+      <c r="AX34" s="39"/>
+      <c r="AY34" s="39">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AZ34" s="35">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="BA34" s="35">
+        <f t="shared" ref="BA34:BA36" si="16">G34-AZ34</f>
+        <v>0</v>
+      </c>
+      <c r="BB34" s="2"/>
+    </row>
+    <row r="35" spans="2:54" s="41" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="39"/>
+      <c r="N35" s="39"/>
+      <c r="O35" s="39"/>
+      <c r="P35" s="39"/>
+      <c r="Q35" s="39"/>
+      <c r="R35" s="39"/>
+      <c r="S35" s="39"/>
+      <c r="T35" s="39"/>
+      <c r="U35" s="39"/>
+      <c r="V35" s="39"/>
+      <c r="W35" s="39"/>
+      <c r="X35" s="39"/>
+      <c r="Y35" s="39"/>
+      <c r="Z35" s="39"/>
+      <c r="AA35" s="39"/>
+      <c r="AB35" s="39"/>
+      <c r="AC35" s="39"/>
+      <c r="AD35" s="39"/>
+      <c r="AE35" s="39"/>
+      <c r="AF35" s="39"/>
+      <c r="AG35" s="39"/>
+      <c r="AH35" s="39"/>
+      <c r="AI35" s="39"/>
+      <c r="AJ35" s="39"/>
+      <c r="AK35" s="39"/>
+      <c r="AL35" s="39"/>
+      <c r="AM35" s="39"/>
+      <c r="AN35" s="39"/>
+      <c r="AO35" s="39"/>
+      <c r="AP35" s="39"/>
+      <c r="AQ35" s="39"/>
+      <c r="AR35" s="39"/>
+      <c r="AS35" s="39"/>
+      <c r="AT35" s="39"/>
+      <c r="AU35" s="39"/>
+      <c r="AV35" s="39"/>
+      <c r="AW35" s="39"/>
+      <c r="AX35" s="39"/>
+      <c r="AY35" s="39"/>
+      <c r="AZ35" s="35"/>
+      <c r="BA35" s="35"/>
+      <c r="BB35" s="2"/>
+    </row>
+    <row r="36" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="42"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="G36" s="43">
+        <v>2</v>
+      </c>
+      <c r="H36" s="39"/>
+      <c r="I36" s="39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J36" s="39"/>
+      <c r="K36" s="39"/>
+      <c r="L36" s="39">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M36" s="39"/>
+      <c r="N36" s="39"/>
+      <c r="O36" s="39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P36" s="39"/>
+      <c r="Q36" s="39"/>
+      <c r="R36" s="39">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="S36" s="39"/>
+      <c r="T36" s="39">
+        <v>1</v>
+      </c>
+      <c r="U36" s="39">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="V36" s="39"/>
+      <c r="W36" s="39"/>
+      <c r="X36" s="39">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Y36" s="39"/>
+      <c r="Z36" s="39"/>
+      <c r="AA36" s="39">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AB36" s="39"/>
+      <c r="AC36" s="39"/>
+      <c r="AD36" s="39">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="AE36" s="39"/>
+      <c r="AF36" s="39"/>
+      <c r="AG36" s="39">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AH36" s="39"/>
+      <c r="AI36" s="39"/>
+      <c r="AJ36" s="39">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="AK36" s="39"/>
+      <c r="AL36" s="39"/>
+      <c r="AM36" s="39">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AN36" s="39"/>
+      <c r="AO36" s="39"/>
+      <c r="AP36" s="39">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AQ36" s="39"/>
+      <c r="AR36" s="39"/>
+      <c r="AS36" s="39">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AT36" s="39"/>
+      <c r="AU36" s="39"/>
+      <c r="AV36" s="39">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AW36" s="39"/>
+      <c r="AX36" s="39"/>
+      <c r="AY36" s="39">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="AZ36" s="35">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="BA36" s="35">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="BB36" s="2"/>
+    </row>
+    <row r="37" spans="2:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="45"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="14"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="15"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="14"/>
+      <c r="AB37" s="15"/>
+      <c r="AC37" s="14"/>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="15"/>
+      <c r="AF37" s="14"/>
+      <c r="AG37" s="14"/>
+      <c r="AH37" s="15"/>
+      <c r="AI37" s="14"/>
+      <c r="AJ37" s="14"/>
+      <c r="AK37" s="15"/>
+      <c r="AL37" s="14"/>
+      <c r="AM37" s="14"/>
+      <c r="AN37" s="15"/>
+      <c r="AO37" s="14"/>
+      <c r="AP37" s="14"/>
+      <c r="AQ37" s="15"/>
+      <c r="AR37" s="14"/>
+      <c r="AS37" s="14"/>
+      <c r="AT37" s="15"/>
+      <c r="AU37" s="14"/>
+      <c r="AV37" s="14"/>
+      <c r="AW37" s="15"/>
+      <c r="AX37" s="14"/>
+      <c r="AY37" s="14"/>
+      <c r="AZ37" s="14"/>
+      <c r="BA37" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3820,6 +4312,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -3839,7 +4336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A2" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CU 01 y 25
Se agregaron los diagramas de los dos casos de uso correspondientes a esta iteración, se corrigieron descripciones, se realizó la interfaz gráfica de ambos CU y se empezó con la codificación del CU-25 Mostrar información de renta
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 5/Plantilla Lista de Tareas de la Entrega 5.xlsx
+++ b/Plantillas/Entrega 5/Plantilla Lista de Tareas de la Entrega 5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3085F081-C115-42DC-89A9-72B5B4CD5E97}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E3A7BA-44E5-460B-8E0C-10DC259B3E9E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -911,10 +911,10 @@
   <dimension ref="B1:BB43"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AI6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AU29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AJ17" sqref="AJ17"/>
+      <selection pane="bottomRight" activeCell="AZ33" sqref="AZ33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3622,7 +3622,7 @@
         <v>42</v>
       </c>
       <c r="F31" s="42" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G31" s="43">
         <v>2</v>
@@ -3689,42 +3689,44 @@
         <v>1</v>
       </c>
       <c r="AK31" s="39"/>
-      <c r="AL31" s="39"/>
+      <c r="AL31" s="39">
+        <v>0.5</v>
+      </c>
       <c r="AM31" s="39">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AN31" s="39"/>
       <c r="AO31" s="39"/>
       <c r="AP31" s="39">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AQ31" s="39"/>
       <c r="AR31" s="39"/>
       <c r="AS31" s="39">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AT31" s="39"/>
       <c r="AU31" s="39"/>
       <c r="AV31" s="39">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW31" s="39"/>
       <c r="AX31" s="39"/>
       <c r="AY31" s="39">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AZ31" s="35">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="BA31" s="35">
         <f>G31-AZ31</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="BB31" s="2"/>
     </row>
@@ -3738,7 +3740,7 @@
         <v>42</v>
       </c>
       <c r="F32" s="42" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G32" s="43">
         <v>2</v>
@@ -3805,42 +3807,44 @@
         <v>1</v>
       </c>
       <c r="AK32" s="39"/>
-      <c r="AL32" s="39"/>
+      <c r="AL32" s="39">
+        <v>0.5</v>
+      </c>
       <c r="AM32" s="39">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AN32" s="39"/>
       <c r="AO32" s="39"/>
       <c r="AP32" s="39">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AQ32" s="39"/>
       <c r="AR32" s="39"/>
       <c r="AS32" s="39">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AT32" s="39"/>
       <c r="AU32" s="39"/>
       <c r="AV32" s="39">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW32" s="39"/>
       <c r="AX32" s="39"/>
       <c r="AY32" s="39">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AZ32" s="35">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="BA32" s="35">
         <f>G32-AZ32</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="BB32" s="2"/>
     </row>
@@ -4029,7 +4033,7 @@
         <v>42</v>
       </c>
       <c r="F35" s="39" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G35" s="43">
         <v>2</v>
@@ -4096,42 +4100,44 @@
         <v>1</v>
       </c>
       <c r="AK35" s="39"/>
-      <c r="AL35" s="39"/>
+      <c r="AL35" s="39">
+        <v>0.5</v>
+      </c>
       <c r="AM35" s="39">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AN35" s="39"/>
       <c r="AO35" s="39"/>
       <c r="AP35" s="39">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AQ35" s="39"/>
       <c r="AR35" s="39"/>
       <c r="AS35" s="39">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AT35" s="39"/>
       <c r="AU35" s="39"/>
       <c r="AV35" s="39">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW35" s="39"/>
       <c r="AX35" s="39"/>
       <c r="AY35" s="39">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AZ35" s="35">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="BA35" s="35">
         <f>G35-AZ35</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="BB35" s="2"/>
     </row>
@@ -4145,7 +4151,7 @@
         <v>42</v>
       </c>
       <c r="F36" s="39" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G36" s="43">
         <v>2</v>
@@ -4212,42 +4218,44 @@
         <v>1</v>
       </c>
       <c r="AK36" s="39"/>
-      <c r="AL36" s="39"/>
+      <c r="AL36" s="39">
+        <v>0.5</v>
+      </c>
       <c r="AM36" s="39">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AN36" s="39"/>
       <c r="AO36" s="39"/>
       <c r="AP36" s="39">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AQ36" s="39"/>
       <c r="AR36" s="39"/>
       <c r="AS36" s="39">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AT36" s="39"/>
       <c r="AU36" s="39"/>
       <c r="AV36" s="39">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW36" s="39"/>
       <c r="AX36" s="39"/>
       <c r="AY36" s="39">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AZ36" s="35">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="BA36" s="35">
         <f>G36-AZ36</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="BB36" s="2"/>
     </row>
@@ -4261,7 +4269,7 @@
         <v>42</v>
       </c>
       <c r="F37" s="39" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G37" s="43">
         <v>2</v>
@@ -4377,7 +4385,7 @@
         <v>42</v>
       </c>
       <c r="F38" s="39" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="G38" s="43">
         <v>4</v>
@@ -4442,42 +4450,44 @@
         <v>4</v>
       </c>
       <c r="AK38" s="39"/>
-      <c r="AL38" s="39"/>
+      <c r="AL38" s="39">
+        <v>1</v>
+      </c>
       <c r="AM38" s="39">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AN38" s="39"/>
       <c r="AO38" s="39"/>
       <c r="AP38" s="39">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AQ38" s="39"/>
       <c r="AR38" s="39"/>
       <c r="AS38" s="39">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AT38" s="39"/>
       <c r="AU38" s="39"/>
       <c r="AV38" s="39">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AW38" s="39"/>
       <c r="AX38" s="39"/>
       <c r="AY38" s="39">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AZ38" s="35">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA38" s="35">
         <f>G38-AZ38</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BB38" s="2"/>
     </row>
@@ -4887,6 +4897,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -4898,11 +4913,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Tareas de la quinta entrega
Se realizaron todas las tareas de la plantilla de tareas y se actualizaron dichas plantillas
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 5/Plantilla Lista de Tareas de la Entrega 5.xlsx
+++ b/Plantillas/Entrega 5/Plantilla Lista de Tareas de la Entrega 5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renato\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E3A7BA-44E5-460B-8E0C-10DC259B3E9E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8640E10A-8109-4613-87E0-B953E47172C4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Instructivo" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Casos de Uso'!$A$1:$BB$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Casos de Uso'!$A$1:$BB$50</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="81">
   <si>
     <t>Columna</t>
   </si>
@@ -258,6 +258,24 @@
   </si>
   <si>
     <t>Prueba unitaria</t>
+  </si>
+  <si>
+    <t>CU-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En este caso de uso el Director creará un nuevo Grupo que tomará clases en las instalaciones, a dicho Grupo se le asignaran: un nombre, un Maestro, un monto de inscripción y de mensualidad </t>
+  </si>
+  <si>
+    <t>Correcciones de implementación</t>
+  </si>
+  <si>
+    <t>Correcciones de diseño</t>
+  </si>
+  <si>
+    <t>CU-11</t>
+  </si>
+  <si>
+    <t>En este caso de uso el Director cambia la asignación del nombre del grupo, maestro y montos del grupo que haya seleccionado</t>
   </si>
 </sst>
 </file>
@@ -908,13 +926,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:BB43"/>
+  <dimension ref="B1:BB49"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AU29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AU24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AZ33" sqref="AZ33"/>
+      <selection pane="bottomRight" activeCell="AZ29" sqref="AZ29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +945,7 @@
     <col min="6" max="6" width="11.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" style="16" customWidth="1"/>
     <col min="8" max="8" width="6.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.7109375" style="2" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -1278,85 +1296,85 @@
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14">
-        <f t="shared" ref="I7:I42" si="0">G7-H7</f>
+        <f t="shared" ref="I7:I48" si="0">G7-H7</f>
         <v>2</v>
       </c>
       <c r="J7" s="15"/>
       <c r="K7" s="14"/>
       <c r="L7" s="14">
-        <f t="shared" ref="L7:L42" si="1">I7-K7</f>
+        <f t="shared" ref="L7:L48" si="1">I7-K7</f>
         <v>2</v>
       </c>
       <c r="M7" s="15"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14">
-        <f t="shared" ref="O7:O42" si="2">L7-N7</f>
+        <f t="shared" ref="O7:O48" si="2">L7-N7</f>
         <v>2</v>
       </c>
       <c r="P7" s="15"/>
       <c r="Q7" s="14"/>
       <c r="R7" s="14">
-        <f t="shared" ref="R7:R42" si="3">O7-Q7</f>
+        <f t="shared" ref="R7:R48" si="3">O7-Q7</f>
         <v>2</v>
       </c>
       <c r="S7" s="15"/>
       <c r="T7" s="14"/>
       <c r="U7" s="14">
-        <f t="shared" ref="U7:U42" si="4">R7-T7</f>
+        <f t="shared" ref="U7:U48" si="4">R7-T7</f>
         <v>2</v>
       </c>
       <c r="V7" s="14"/>
       <c r="W7" s="14"/>
       <c r="X7" s="14">
-        <f t="shared" ref="X7:X42" si="5">U7-W7</f>
+        <f t="shared" ref="X7:X48" si="5">U7-W7</f>
         <v>2</v>
       </c>
       <c r="Y7" s="14"/>
       <c r="Z7" s="14"/>
       <c r="AA7" s="14">
-        <f t="shared" ref="AA7:AA42" si="6">X7-Z7</f>
+        <f t="shared" ref="AA7:AA48" si="6">X7-Z7</f>
         <v>2</v>
       </c>
       <c r="AB7" s="14"/>
       <c r="AC7" s="14"/>
       <c r="AD7" s="14">
-        <f t="shared" ref="AD7:AD42" si="7">AA7-AC7</f>
+        <f t="shared" ref="AD7:AD48" si="7">AA7-AC7</f>
         <v>2</v>
       </c>
       <c r="AE7" s="14"/>
       <c r="AF7" s="14"/>
       <c r="AG7" s="14">
-        <f t="shared" ref="AG7:AG42" si="8">AD7-AF7</f>
+        <f t="shared" ref="AG7:AG48" si="8">AD7-AF7</f>
         <v>2</v>
       </c>
       <c r="AH7" s="14"/>
       <c r="AI7" s="14"/>
       <c r="AJ7" s="14">
-        <f t="shared" ref="AJ7:AJ42" si="9">AG7-AI7</f>
+        <f t="shared" ref="AJ7:AJ48" si="9">AG7-AI7</f>
         <v>2</v>
       </c>
       <c r="AK7" s="14"/>
       <c r="AL7" s="14"/>
       <c r="AM7" s="14">
-        <f t="shared" ref="AM7:AM42" si="10">AJ7-AL7</f>
+        <f t="shared" ref="AM7:AM48" si="10">AJ7-AL7</f>
         <v>2</v>
       </c>
       <c r="AN7" s="14"/>
       <c r="AO7" s="14"/>
       <c r="AP7" s="14">
-        <f t="shared" ref="AP7:AP42" si="11">AM7-AO7</f>
+        <f t="shared" ref="AP7:AP48" si="11">AM7-AO7</f>
         <v>2</v>
       </c>
       <c r="AQ7" s="14"/>
       <c r="AR7" s="14"/>
       <c r="AS7" s="14">
-        <f t="shared" ref="AS7:AS42" si="12">AP7-AR7</f>
+        <f t="shared" ref="AS7:AS48" si="12">AP7-AR7</f>
         <v>2</v>
       </c>
       <c r="AT7" s="14"/>
       <c r="AU7" s="14"/>
       <c r="AV7" s="14">
-        <f t="shared" ref="AV7:AV42" si="13">AS7-AU7</f>
+        <f t="shared" ref="AV7:AV48" si="13">AS7-AU7</f>
         <v>2</v>
       </c>
       <c r="AW7" s="14"/>
@@ -1540,7 +1558,7 @@
         <v>1</v>
       </c>
       <c r="AZ9" s="35">
-        <f t="shared" ref="AZ9:AZ42" si="14">H9+K9+N9+Q9+T9+W9+Z9+AC9+AF9+AI9+AL9+AO9+AR9+AU9+AX9</f>
+        <f t="shared" ref="AZ9:AZ48" si="14">H9+K9+N9+Q9+T9+W9+Z9+AC9+AF9+AI9+AL9+AO9+AR9+AU9+AX9</f>
         <v>1</v>
       </c>
       <c r="BA9" s="35">
@@ -1652,7 +1670,7 @@
       <c r="AW10" s="22"/>
       <c r="AX10" s="22"/>
       <c r="AY10" s="22">
-        <f t="shared" ref="AY10:AY42" si="15">AV10-AX10</f>
+        <f t="shared" ref="AY10:AY48" si="15">AV10-AX10</f>
         <v>1</v>
       </c>
       <c r="AZ10" s="35">
@@ -2820,7 +2838,7 @@
         <v>40</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G23" s="34">
         <v>2</v>
@@ -2903,24 +2921,26 @@
         <v>2</v>
       </c>
       <c r="AT23" s="30"/>
-      <c r="AU23" s="30"/>
+      <c r="AU23" s="30">
+        <v>1</v>
+      </c>
       <c r="AV23" s="30">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW23" s="30"/>
       <c r="AX23" s="30"/>
       <c r="AY23" s="30">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ23" s="35">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA23" s="35">
         <f>G23-AZ23</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB23" s="2"/>
     </row>
@@ -2934,7 +2954,7 @@
         <v>40</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G24" s="34">
         <v>2</v>
@@ -3017,24 +3037,26 @@
         <v>2</v>
       </c>
       <c r="AT24" s="30"/>
-      <c r="AU24" s="30"/>
+      <c r="AU24" s="30">
+        <v>1</v>
+      </c>
       <c r="AV24" s="30">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW24" s="30"/>
       <c r="AX24" s="30"/>
       <c r="AY24" s="30">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ24" s="35">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA24" s="35">
         <f>G24-AZ24</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB24" s="2"/>
     </row>
@@ -3048,107 +3070,109 @@
         <v>40</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G25" s="34">
         <v>2</v>
       </c>
-      <c r="H25" s="30"/>
+      <c r="H25" s="30">
+        <v>2</v>
+      </c>
       <c r="I25" s="30">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J25" s="30"/>
       <c r="K25" s="30"/>
       <c r="L25" s="30">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M25" s="30"/>
       <c r="N25" s="30"/>
       <c r="O25" s="30">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P25" s="30"/>
       <c r="Q25" s="30"/>
       <c r="R25" s="30">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S25" s="30"/>
       <c r="T25" s="30"/>
       <c r="U25" s="30">
         <f>R25-T25</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V25" s="30"/>
       <c r="W25" s="30"/>
       <c r="X25" s="30">
         <f>U25-W25</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y25" s="30"/>
       <c r="Z25" s="30"/>
       <c r="AA25" s="30">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB25" s="30"/>
       <c r="AC25" s="30"/>
       <c r="AD25" s="30">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE25" s="30"/>
       <c r="AF25" s="30"/>
       <c r="AG25" s="30">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH25" s="30"/>
       <c r="AI25" s="30"/>
       <c r="AJ25" s="30">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK25" s="30"/>
       <c r="AL25" s="30"/>
       <c r="AM25" s="30">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN25" s="30"/>
       <c r="AO25" s="30"/>
       <c r="AP25" s="30">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ25" s="30"/>
       <c r="AR25" s="30"/>
       <c r="AS25" s="30">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT25" s="30"/>
       <c r="AU25" s="30"/>
       <c r="AV25" s="30">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW25" s="30"/>
       <c r="AX25" s="30"/>
       <c r="AY25" s="30">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ25" s="35">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA25" s="35">
         <f>G25-AZ25</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BB25" s="2"/>
     </row>
@@ -3221,7 +3245,7 @@
         <v>40</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G27" s="34">
         <v>2</v>
@@ -3298,30 +3322,32 @@
         <v>2</v>
       </c>
       <c r="AQ27" s="30"/>
-      <c r="AR27" s="30"/>
+      <c r="AR27" s="30">
+        <v>1</v>
+      </c>
       <c r="AS27" s="30">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT27" s="30"/>
       <c r="AU27" s="30"/>
       <c r="AV27" s="30">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW27" s="30"/>
       <c r="AX27" s="30"/>
       <c r="AY27" s="30">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ27" s="35">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA27" s="35">
         <f>G27-AZ27</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB27" s="2"/>
     </row>
@@ -3335,7 +3361,7 @@
         <v>40</v>
       </c>
       <c r="F28" s="30" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G28" s="34">
         <v>2</v>
@@ -3412,30 +3438,32 @@
         <v>2</v>
       </c>
       <c r="AQ28" s="30"/>
-      <c r="AR28" s="30"/>
+      <c r="AR28" s="30">
+        <v>1</v>
+      </c>
       <c r="AS28" s="30">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT28" s="30"/>
       <c r="AU28" s="30"/>
       <c r="AV28" s="30">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW28" s="30"/>
       <c r="AX28" s="30"/>
       <c r="AY28" s="30">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ28" s="35">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA28" s="35">
         <f>G28-AZ28</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB28" s="2"/>
     </row>
@@ -3449,20 +3477,20 @@
         <v>40</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G29" s="34">
         <v>2</v>
       </c>
       <c r="H29" s="30"/>
       <c r="I29" s="30">
-        <f t="shared" si="0"/>
+        <f>G29-H29</f>
         <v>2</v>
       </c>
       <c r="J29" s="30"/>
       <c r="K29" s="30"/>
       <c r="L29" s="30">
-        <f t="shared" si="1"/>
+        <f>I29-K29</f>
         <v>2</v>
       </c>
       <c r="M29" s="30"/>
@@ -3526,749 +3554,686 @@
         <v>2</v>
       </c>
       <c r="AQ29" s="30"/>
-      <c r="AR29" s="30"/>
+      <c r="AR29" s="30">
+        <v>2</v>
+      </c>
       <c r="AS29" s="30">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT29" s="30"/>
       <c r="AU29" s="30"/>
       <c r="AV29" s="30">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW29" s="30"/>
       <c r="AX29" s="30"/>
       <c r="AY29" s="30">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ29" s="35">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA29" s="35">
         <f>G29-AZ29</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BB29" s="2"/>
     </row>
-    <row r="30" spans="2:54" s="41" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39"/>
-      <c r="O30" s="39"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="39"/>
-      <c r="R30" s="39"/>
-      <c r="S30" s="39"/>
-      <c r="T30" s="39"/>
-      <c r="U30" s="39"/>
-      <c r="V30" s="39"/>
-      <c r="W30" s="39"/>
-      <c r="X30" s="39"/>
-      <c r="Y30" s="39"/>
-      <c r="Z30" s="39"/>
-      <c r="AA30" s="39"/>
-      <c r="AB30" s="39"/>
-      <c r="AC30" s="39"/>
-      <c r="AD30" s="39"/>
-      <c r="AE30" s="39"/>
-      <c r="AF30" s="39"/>
-      <c r="AG30" s="39"/>
-      <c r="AH30" s="39"/>
-      <c r="AI30" s="39"/>
-      <c r="AJ30" s="39"/>
-      <c r="AK30" s="39"/>
-      <c r="AL30" s="39"/>
-      <c r="AM30" s="39"/>
-      <c r="AN30" s="39"/>
-      <c r="AO30" s="39"/>
-      <c r="AP30" s="39"/>
-      <c r="AQ30" s="39"/>
-      <c r="AR30" s="39"/>
-      <c r="AS30" s="39"/>
-      <c r="AT30" s="39"/>
-      <c r="AU30" s="39"/>
-      <c r="AV30" s="39"/>
-      <c r="AW30" s="39"/>
-      <c r="AX30" s="39"/>
-      <c r="AY30" s="39"/>
+    <row r="30" spans="2:54" s="32" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="27"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="30"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="30"/>
+      <c r="T30" s="30"/>
+      <c r="U30" s="30"/>
+      <c r="V30" s="30"/>
+      <c r="W30" s="30"/>
+      <c r="X30" s="30"/>
+      <c r="Y30" s="30"/>
+      <c r="Z30" s="30"/>
+      <c r="AA30" s="30"/>
+      <c r="AB30" s="30"/>
+      <c r="AC30" s="30"/>
+      <c r="AD30" s="30"/>
+      <c r="AE30" s="30"/>
+      <c r="AF30" s="30"/>
+      <c r="AG30" s="30"/>
+      <c r="AH30" s="30"/>
+      <c r="AI30" s="30"/>
+      <c r="AJ30" s="30"/>
+      <c r="AK30" s="30"/>
+      <c r="AL30" s="30"/>
+      <c r="AM30" s="30"/>
+      <c r="AN30" s="30"/>
+      <c r="AO30" s="30"/>
+      <c r="AP30" s="30"/>
+      <c r="AQ30" s="30"/>
+      <c r="AR30" s="30"/>
+      <c r="AS30" s="30"/>
+      <c r="AT30" s="30"/>
+      <c r="AU30" s="30"/>
+      <c r="AV30" s="30"/>
+      <c r="AW30" s="30"/>
+      <c r="AX30" s="30"/>
+      <c r="AY30" s="30"/>
       <c r="AZ30" s="35"/>
       <c r="BA30" s="35"/>
       <c r="BB30" s="2"/>
     </row>
-    <row r="31" spans="2:54" s="41" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="42"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="42" t="s">
+    <row r="31" spans="2:54" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="33"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="G31" s="43">
-        <v>2</v>
-      </c>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M31" s="39"/>
-      <c r="N31" s="39"/>
-      <c r="O31" s="39">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="39"/>
-      <c r="R31" s="39">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="S31" s="39"/>
-      <c r="T31" s="39"/>
-      <c r="U31" s="39">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="V31" s="39"/>
-      <c r="W31" s="39"/>
-      <c r="X31" s="39">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Y31" s="39"/>
-      <c r="Z31" s="39">
-        <v>1</v>
-      </c>
-      <c r="AA31" s="39">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="AB31" s="39"/>
-      <c r="AC31" s="39"/>
-      <c r="AD31" s="39">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AE31" s="39"/>
-      <c r="AF31" s="39"/>
-      <c r="AG31" s="39">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="AH31" s="39"/>
-      <c r="AI31" s="39"/>
-      <c r="AJ31" s="39">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AK31" s="39"/>
-      <c r="AL31" s="39">
-        <v>0.5</v>
-      </c>
-      <c r="AM31" s="39">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="AN31" s="39"/>
-      <c r="AO31" s="39"/>
-      <c r="AP31" s="39">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="AQ31" s="39"/>
-      <c r="AR31" s="39"/>
-      <c r="AS31" s="39">
-        <f t="shared" si="12"/>
-        <v>0.5</v>
-      </c>
-      <c r="AT31" s="39"/>
-      <c r="AU31" s="39"/>
-      <c r="AV31" s="39">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="AW31" s="39"/>
-      <c r="AX31" s="39"/>
-      <c r="AY31" s="39">
-        <f t="shared" si="15"/>
-        <v>0.5</v>
+      <c r="G31" s="34">
+        <v>2</v>
+      </c>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30">
+        <f>G31-IH31</f>
+        <v>2</v>
+      </c>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30">
+        <v>2</v>
+      </c>
+      <c r="L31" s="30">
+        <f>I31-K31</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30">
+        <f t="shared" ref="O31:O32" si="17">L31-N31</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="30"/>
+      <c r="Q31" s="30"/>
+      <c r="R31" s="30">
+        <f t="shared" ref="R31:R32" si="18">O31-Q31</f>
+        <v>0</v>
+      </c>
+      <c r="S31" s="30"/>
+      <c r="T31" s="30"/>
+      <c r="U31" s="30">
+        <f t="shared" ref="U31:U32" si="19">R31-T31</f>
+        <v>0</v>
+      </c>
+      <c r="V31" s="30"/>
+      <c r="W31" s="30"/>
+      <c r="X31" s="30">
+        <f t="shared" ref="X31:X32" si="20">U31-W31</f>
+        <v>0</v>
+      </c>
+      <c r="Y31" s="30"/>
+      <c r="Z31" s="30"/>
+      <c r="AA31" s="30">
+        <f t="shared" ref="AA31:AA32" si="21">X31-Z31</f>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="30"/>
+      <c r="AC31" s="30"/>
+      <c r="AD31" s="30">
+        <f t="shared" ref="AD31:AD32" si="22">AA31-AC31</f>
+        <v>0</v>
+      </c>
+      <c r="AE31" s="30"/>
+      <c r="AF31" s="30"/>
+      <c r="AG31" s="30">
+        <f t="shared" ref="AG31:AG32" si="23">AD31-AF31</f>
+        <v>0</v>
+      </c>
+      <c r="AH31" s="30"/>
+      <c r="AI31" s="30"/>
+      <c r="AJ31" s="30">
+        <f t="shared" ref="AJ31:AJ32" si="24">AG31-AI31</f>
+        <v>0</v>
+      </c>
+      <c r="AK31" s="30"/>
+      <c r="AL31" s="30"/>
+      <c r="AM31" s="30">
+        <f t="shared" ref="AM31:AM32" si="25">AJ31-AL31</f>
+        <v>0</v>
+      </c>
+      <c r="AN31" s="30"/>
+      <c r="AO31" s="30"/>
+      <c r="AP31" s="30">
+        <f t="shared" ref="AP31:AP32" si="26">AM31-AO31</f>
+        <v>0</v>
+      </c>
+      <c r="AQ31" s="30"/>
+      <c r="AR31" s="30"/>
+      <c r="AS31" s="30">
+        <f t="shared" ref="AS31:AS32" si="27">AP31-AR31</f>
+        <v>0</v>
+      </c>
+      <c r="AT31" s="30"/>
+      <c r="AU31" s="30"/>
+      <c r="AV31" s="30">
+        <f t="shared" ref="AV31:AV32" si="28">AS31-AU31</f>
+        <v>0</v>
+      </c>
+      <c r="AW31" s="30"/>
+      <c r="AX31" s="30"/>
+      <c r="AY31" s="30">
+        <f t="shared" ref="AY31:AY32" si="29">AV31-AX31</f>
+        <v>0</v>
       </c>
       <c r="AZ31" s="35">
         <f t="shared" si="14"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="BA31" s="35">
-        <f>G31-AZ31</f>
-        <v>0.5</v>
+        <f t="shared" ref="BA30:BA35" si="30">G31-AZ31</f>
+        <v>0</v>
       </c>
       <c r="BB31" s="2"/>
     </row>
-    <row r="32" spans="2:54" s="41" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="42"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="42" t="s">
+    <row r="32" spans="2:54" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="33"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="43">
-        <v>2</v>
-      </c>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M32" s="39"/>
-      <c r="N32" s="39"/>
-      <c r="O32" s="39">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="P32" s="39"/>
-      <c r="Q32" s="39"/>
-      <c r="R32" s="39">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="S32" s="39"/>
-      <c r="T32" s="39"/>
-      <c r="U32" s="39">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="V32" s="39"/>
-      <c r="W32" s="39"/>
-      <c r="X32" s="39">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Y32" s="39"/>
-      <c r="Z32" s="39">
-        <v>1</v>
-      </c>
-      <c r="AA32" s="39">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="AB32" s="39"/>
-      <c r="AC32" s="39"/>
-      <c r="AD32" s="39">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AE32" s="39"/>
-      <c r="AF32" s="39"/>
-      <c r="AG32" s="39">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="AH32" s="39"/>
-      <c r="AI32" s="39"/>
-      <c r="AJ32" s="39">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AK32" s="39"/>
-      <c r="AL32" s="39">
-        <v>0.5</v>
-      </c>
-      <c r="AM32" s="39">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="AN32" s="39"/>
-      <c r="AO32" s="39"/>
-      <c r="AP32" s="39">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="AQ32" s="39"/>
-      <c r="AR32" s="39"/>
-      <c r="AS32" s="39">
-        <f t="shared" si="12"/>
-        <v>0.5</v>
-      </c>
-      <c r="AT32" s="39"/>
-      <c r="AU32" s="39"/>
-      <c r="AV32" s="39">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="AW32" s="39"/>
-      <c r="AX32" s="39"/>
-      <c r="AY32" s="39">
-        <f t="shared" si="15"/>
-        <v>0.5</v>
+      <c r="G32" s="34">
+        <v>1</v>
+      </c>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30">
+        <f>G32-H32</f>
+        <v>1</v>
+      </c>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30">
+        <f>I32-K32</f>
+        <v>1</v>
+      </c>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="30">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="S32" s="30"/>
+      <c r="T32" s="30"/>
+      <c r="U32" s="30">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="V32" s="30"/>
+      <c r="W32" s="30"/>
+      <c r="X32" s="30">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="Y32" s="30"/>
+      <c r="Z32" s="30"/>
+      <c r="AA32" s="30">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AB32" s="30"/>
+      <c r="AC32" s="30"/>
+      <c r="AD32" s="30">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AE32" s="30"/>
+      <c r="AF32" s="30"/>
+      <c r="AG32" s="30">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="AH32" s="30"/>
+      <c r="AI32" s="30">
+        <v>1</v>
+      </c>
+      <c r="AJ32" s="30">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AK32" s="30"/>
+      <c r="AL32" s="30"/>
+      <c r="AM32" s="30">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="AN32" s="30"/>
+      <c r="AO32" s="30"/>
+      <c r="AP32" s="30">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="AQ32" s="30"/>
+      <c r="AR32" s="30"/>
+      <c r="AS32" s="30">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="AT32" s="30"/>
+      <c r="AU32" s="30"/>
+      <c r="AV32" s="30">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AW32" s="30"/>
+      <c r="AX32" s="30"/>
+      <c r="AY32" s="30">
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AZ32" s="35">
         <f t="shared" si="14"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="BA32" s="35">
-        <f>G32-AZ32</f>
-        <v>0.5</v>
+        <f t="shared" si="30"/>
+        <v>0</v>
       </c>
       <c r="BB32" s="2"/>
     </row>
-    <row r="33" spans="2:54" s="41" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="42"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="F33" s="42" t="s">
+    <row r="33" spans="2:54" s="32" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="27"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="30"/>
+      <c r="Q33" s="30"/>
+      <c r="R33" s="30"/>
+      <c r="S33" s="30"/>
+      <c r="T33" s="30"/>
+      <c r="U33" s="30"/>
+      <c r="V33" s="30"/>
+      <c r="W33" s="30"/>
+      <c r="X33" s="30"/>
+      <c r="Y33" s="30"/>
+      <c r="Z33" s="30"/>
+      <c r="AA33" s="30"/>
+      <c r="AB33" s="30"/>
+      <c r="AC33" s="30"/>
+      <c r="AD33" s="30"/>
+      <c r="AE33" s="30"/>
+      <c r="AF33" s="30"/>
+      <c r="AG33" s="30"/>
+      <c r="AH33" s="30"/>
+      <c r="AI33" s="30"/>
+      <c r="AJ33" s="30"/>
+      <c r="AK33" s="30"/>
+      <c r="AL33" s="30"/>
+      <c r="AM33" s="30"/>
+      <c r="AN33" s="30"/>
+      <c r="AO33" s="30"/>
+      <c r="AP33" s="30"/>
+      <c r="AQ33" s="30"/>
+      <c r="AR33" s="30"/>
+      <c r="AS33" s="30"/>
+      <c r="AT33" s="30"/>
+      <c r="AU33" s="30"/>
+      <c r="AV33" s="30"/>
+      <c r="AW33" s="30"/>
+      <c r="AX33" s="30"/>
+      <c r="AY33" s="30"/>
+      <c r="AZ33" s="35"/>
+      <c r="BA33" s="35"/>
+      <c r="BB33" s="2"/>
+    </row>
+    <row r="34" spans="2:54" s="32" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="33"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="43">
-        <v>2</v>
-      </c>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M33" s="39"/>
-      <c r="N33" s="39"/>
-      <c r="O33" s="39">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="P33" s="39"/>
-      <c r="Q33" s="39"/>
-      <c r="R33" s="39">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="S33" s="39"/>
-      <c r="T33" s="39"/>
-      <c r="U33" s="39">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="V33" s="39"/>
-      <c r="W33" s="39"/>
-      <c r="X33" s="39">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="Y33" s="39"/>
-      <c r="Z33" s="39">
-        <v>2</v>
-      </c>
-      <c r="AA33" s="39">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AB33" s="39"/>
-      <c r="AC33" s="39"/>
-      <c r="AD33" s="39">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AE33" s="39"/>
-      <c r="AF33" s="39"/>
-      <c r="AG33" s="39">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AH33" s="39"/>
-      <c r="AI33" s="39"/>
-      <c r="AJ33" s="39">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AK33" s="39"/>
-      <c r="AL33" s="39"/>
-      <c r="AM33" s="39">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AN33" s="39"/>
-      <c r="AO33" s="39"/>
-      <c r="AP33" s="39">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AQ33" s="39"/>
-      <c r="AR33" s="39"/>
-      <c r="AS33" s="39">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AT33" s="39"/>
-      <c r="AU33" s="39"/>
-      <c r="AV33" s="39">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AW33" s="39"/>
-      <c r="AX33" s="39"/>
-      <c r="AY33" s="39">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AZ33" s="35">
+      <c r="G34" s="34">
+        <v>2</v>
+      </c>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30">
+        <f>G34-IH34</f>
+        <v>2</v>
+      </c>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30">
+        <f>I34-K34</f>
+        <v>2</v>
+      </c>
+      <c r="M34" s="30"/>
+      <c r="N34" s="30">
+        <v>2</v>
+      </c>
+      <c r="O34" s="30">
+        <f t="shared" ref="O34:O35" si="31">L34-N34</f>
+        <v>0</v>
+      </c>
+      <c r="P34" s="30"/>
+      <c r="Q34" s="30"/>
+      <c r="R34" s="30">
+        <f t="shared" ref="R34:R35" si="32">O34-Q34</f>
+        <v>0</v>
+      </c>
+      <c r="S34" s="30"/>
+      <c r="T34" s="30"/>
+      <c r="U34" s="30">
+        <f t="shared" ref="U34:U35" si="33">R34-T34</f>
+        <v>0</v>
+      </c>
+      <c r="V34" s="30"/>
+      <c r="W34" s="30"/>
+      <c r="X34" s="30">
+        <f t="shared" ref="X34:X35" si="34">U34-W34</f>
+        <v>0</v>
+      </c>
+      <c r="Y34" s="30"/>
+      <c r="Z34" s="30"/>
+      <c r="AA34" s="30">
+        <f t="shared" ref="AA34:AA35" si="35">X34-Z34</f>
+        <v>0</v>
+      </c>
+      <c r="AB34" s="30"/>
+      <c r="AC34" s="30"/>
+      <c r="AD34" s="30">
+        <f t="shared" ref="AD34:AD35" si="36">AA34-AC34</f>
+        <v>0</v>
+      </c>
+      <c r="AE34" s="30"/>
+      <c r="AF34" s="30"/>
+      <c r="AG34" s="30">
+        <f t="shared" ref="AG34:AG35" si="37">AD34-AF34</f>
+        <v>0</v>
+      </c>
+      <c r="AH34" s="30"/>
+      <c r="AI34" s="30"/>
+      <c r="AJ34" s="30">
+        <f t="shared" ref="AJ34:AJ35" si="38">AG34-AI34</f>
+        <v>0</v>
+      </c>
+      <c r="AK34" s="30"/>
+      <c r="AL34" s="30"/>
+      <c r="AM34" s="30">
+        <f t="shared" ref="AM34:AM35" si="39">AJ34-AL34</f>
+        <v>0</v>
+      </c>
+      <c r="AN34" s="30"/>
+      <c r="AO34" s="30"/>
+      <c r="AP34" s="30">
+        <f t="shared" ref="AP34:AP35" si="40">AM34-AO34</f>
+        <v>0</v>
+      </c>
+      <c r="AQ34" s="30"/>
+      <c r="AR34" s="30"/>
+      <c r="AS34" s="30">
+        <f t="shared" ref="AS34:AS35" si="41">AP34-AR34</f>
+        <v>0</v>
+      </c>
+      <c r="AT34" s="30"/>
+      <c r="AU34" s="30"/>
+      <c r="AV34" s="30">
+        <f t="shared" ref="AV34:AV35" si="42">AS34-AU34</f>
+        <v>0</v>
+      </c>
+      <c r="AW34" s="30"/>
+      <c r="AX34" s="30"/>
+      <c r="AY34" s="30">
+        <f t="shared" ref="AY34:AY35" si="43">AV34-AX34</f>
+        <v>0</v>
+      </c>
+      <c r="AZ34" s="35">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="BA33" s="35">
-        <f>G33-AZ33</f>
-        <v>0</v>
-      </c>
-      <c r="BB33" s="2"/>
-    </row>
-    <row r="34" spans="2:54" s="41" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="39"/>
-      <c r="P34" s="39"/>
-      <c r="Q34" s="39"/>
-      <c r="R34" s="39"/>
-      <c r="S34" s="39"/>
-      <c r="T34" s="39"/>
-      <c r="U34" s="39"/>
-      <c r="V34" s="39"/>
-      <c r="W34" s="39"/>
-      <c r="X34" s="39"/>
-      <c r="Y34" s="39"/>
-      <c r="Z34" s="39"/>
-      <c r="AA34" s="39"/>
-      <c r="AB34" s="39"/>
-      <c r="AC34" s="39"/>
-      <c r="AD34" s="39"/>
-      <c r="AE34" s="39"/>
-      <c r="AF34" s="39"/>
-      <c r="AG34" s="39"/>
-      <c r="AH34" s="39"/>
-      <c r="AI34" s="39"/>
-      <c r="AJ34" s="39"/>
-      <c r="AK34" s="39"/>
-      <c r="AL34" s="39"/>
-      <c r="AM34" s="39"/>
-      <c r="AN34" s="39"/>
-      <c r="AO34" s="39"/>
-      <c r="AP34" s="39"/>
-      <c r="AQ34" s="39"/>
-      <c r="AR34" s="39"/>
-      <c r="AS34" s="39"/>
-      <c r="AT34" s="39"/>
-      <c r="AU34" s="39"/>
-      <c r="AV34" s="39"/>
-      <c r="AW34" s="39"/>
-      <c r="AX34" s="39"/>
-      <c r="AY34" s="39"/>
-      <c r="AZ34" s="35"/>
-      <c r="BA34" s="35"/>
+      <c r="BA34" s="35">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
       <c r="BB34" s="2"/>
     </row>
-    <row r="35" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="42"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="E35" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="F35" s="39" t="s">
+    <row r="35" spans="2:54" s="32" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="33"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="G35" s="43">
-        <v>2</v>
-      </c>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
-      <c r="O35" s="39">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="P35" s="39"/>
-      <c r="Q35" s="39"/>
-      <c r="R35" s="39">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="S35" s="39"/>
-      <c r="T35" s="39"/>
-      <c r="U35" s="39">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="V35" s="39"/>
-      <c r="W35" s="39">
-        <v>1</v>
-      </c>
-      <c r="X35" s="39">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Y35" s="39"/>
-      <c r="Z35" s="39"/>
-      <c r="AA35" s="39">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="AB35" s="39"/>
-      <c r="AC35" s="39"/>
-      <c r="AD35" s="39">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AE35" s="39"/>
-      <c r="AF35" s="39"/>
-      <c r="AG35" s="39">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="AH35" s="39"/>
-      <c r="AI35" s="39"/>
-      <c r="AJ35" s="39">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AK35" s="39"/>
-      <c r="AL35" s="39">
-        <v>0.5</v>
-      </c>
-      <c r="AM35" s="39">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="AN35" s="39"/>
-      <c r="AO35" s="39"/>
-      <c r="AP35" s="39">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="AQ35" s="39"/>
-      <c r="AR35" s="39"/>
-      <c r="AS35" s="39">
-        <f t="shared" si="12"/>
-        <v>0.5</v>
-      </c>
-      <c r="AT35" s="39"/>
-      <c r="AU35" s="39"/>
-      <c r="AV35" s="39">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="AW35" s="39"/>
-      <c r="AX35" s="39"/>
-      <c r="AY35" s="39">
-        <f t="shared" si="15"/>
-        <v>0.5</v>
+      <c r="G35" s="34">
+        <v>1</v>
+      </c>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30">
+        <f>G35-H35</f>
+        <v>1</v>
+      </c>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="30">
+        <f>I35-K35</f>
+        <v>1</v>
+      </c>
+      <c r="M35" s="30"/>
+      <c r="N35" s="30"/>
+      <c r="O35" s="30">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="P35" s="30"/>
+      <c r="Q35" s="30"/>
+      <c r="R35" s="30">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="S35" s="30"/>
+      <c r="T35" s="30"/>
+      <c r="U35" s="30">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="V35" s="30"/>
+      <c r="W35" s="30"/>
+      <c r="X35" s="30">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="Y35" s="30"/>
+      <c r="Z35" s="30"/>
+      <c r="AA35" s="30">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+      <c r="AB35" s="30"/>
+      <c r="AC35" s="30"/>
+      <c r="AD35" s="30">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="AE35" s="30"/>
+      <c r="AF35" s="30"/>
+      <c r="AG35" s="30">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="AH35" s="30"/>
+      <c r="AI35" s="30"/>
+      <c r="AJ35" s="30">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="AK35" s="30"/>
+      <c r="AL35" s="30"/>
+      <c r="AM35" s="30">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="AN35" s="30"/>
+      <c r="AO35" s="30"/>
+      <c r="AP35" s="30">
+        <f t="shared" si="40"/>
+        <v>1</v>
+      </c>
+      <c r="AQ35" s="30"/>
+      <c r="AR35" s="30">
+        <v>1</v>
+      </c>
+      <c r="AS35" s="30">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="AT35" s="30"/>
+      <c r="AU35" s="30"/>
+      <c r="AV35" s="30">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="AW35" s="30"/>
+      <c r="AX35" s="30"/>
+      <c r="AY35" s="30">
+        <f t="shared" si="43"/>
+        <v>0</v>
       </c>
       <c r="AZ35" s="35">
         <f t="shared" si="14"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="BA35" s="35">
-        <f>G35-AZ35</f>
-        <v>0.5</v>
+        <f t="shared" si="30"/>
+        <v>0</v>
       </c>
       <c r="BB35" s="2"/>
     </row>
-    <row r="36" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="42"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="G36" s="43">
-        <v>2</v>
-      </c>
+    <row r="36" spans="2:54" s="41" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="40"/>
       <c r="H36" s="39"/>
-      <c r="I36" s="39">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
+      <c r="I36" s="39"/>
       <c r="J36" s="39"/>
       <c r="K36" s="39"/>
-      <c r="L36" s="39">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
+      <c r="L36" s="39"/>
       <c r="M36" s="39"/>
       <c r="N36" s="39"/>
-      <c r="O36" s="39">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
+      <c r="O36" s="39"/>
       <c r="P36" s="39"/>
       <c r="Q36" s="39"/>
-      <c r="R36" s="39">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
+      <c r="R36" s="39"/>
       <c r="S36" s="39"/>
       <c r="T36" s="39"/>
-      <c r="U36" s="39">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
+      <c r="U36" s="39"/>
       <c r="V36" s="39"/>
-      <c r="W36" s="39">
-        <v>1</v>
-      </c>
-      <c r="X36" s="39">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
+      <c r="W36" s="39"/>
+      <c r="X36" s="39"/>
       <c r="Y36" s="39"/>
       <c r="Z36" s="39"/>
-      <c r="AA36" s="39">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
+      <c r="AA36" s="39"/>
       <c r="AB36" s="39"/>
       <c r="AC36" s="39"/>
-      <c r="AD36" s="39">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
+      <c r="AD36" s="39"/>
       <c r="AE36" s="39"/>
       <c r="AF36" s="39"/>
-      <c r="AG36" s="39">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
+      <c r="AG36" s="39"/>
       <c r="AH36" s="39"/>
       <c r="AI36" s="39"/>
-      <c r="AJ36" s="39">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
+      <c r="AJ36" s="39"/>
       <c r="AK36" s="39"/>
-      <c r="AL36" s="39">
-        <v>0.5</v>
-      </c>
-      <c r="AM36" s="39">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
+      <c r="AL36" s="39"/>
+      <c r="AM36" s="39"/>
       <c r="AN36" s="39"/>
       <c r="AO36" s="39"/>
-      <c r="AP36" s="39">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
+      <c r="AP36" s="39"/>
       <c r="AQ36" s="39"/>
       <c r="AR36" s="39"/>
-      <c r="AS36" s="39">
-        <f t="shared" si="12"/>
-        <v>0.5</v>
-      </c>
+      <c r="AS36" s="39"/>
       <c r="AT36" s="39"/>
       <c r="AU36" s="39"/>
-      <c r="AV36" s="39">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
+      <c r="AV36" s="39"/>
       <c r="AW36" s="39"/>
       <c r="AX36" s="39"/>
-      <c r="AY36" s="39">
-        <f t="shared" si="15"/>
-        <v>0.5</v>
-      </c>
-      <c r="AZ36" s="35">
-        <f t="shared" si="14"/>
-        <v>1.5</v>
-      </c>
-      <c r="BA36" s="35">
-        <f>G36-AZ36</f>
-        <v>0.5</v>
-      </c>
+      <c r="AY36" s="39"/>
+      <c r="AZ36" s="35"/>
+      <c r="BA36" s="35"/>
       <c r="BB36" s="2"/>
     </row>
-    <row r="37" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:54" s="41" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="42"/>
       <c r="C37" s="37"/>
       <c r="D37" s="36" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E37" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="F37" s="39" t="s">
+      <c r="F37" s="42" t="s">
         <v>62</v>
       </c>
       <c r="G37" s="43">
@@ -4310,15 +4275,15 @@
         <v>2</v>
       </c>
       <c r="Y37" s="39"/>
-      <c r="Z37" s="39"/>
+      <c r="Z37" s="39">
+        <v>1</v>
+      </c>
       <c r="AA37" s="39">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB37" s="39"/>
-      <c r="AC37" s="39">
-        <v>1</v>
-      </c>
+      <c r="AC37" s="39"/>
       <c r="AD37" s="39">
         <f t="shared" si="7"/>
         <v>1</v>
@@ -4336,400 +4301,463 @@
         <v>1</v>
       </c>
       <c r="AK37" s="39"/>
-      <c r="AL37" s="39"/>
+      <c r="AL37" s="39">
+        <v>0.5</v>
+      </c>
       <c r="AM37" s="39">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AN37" s="39"/>
       <c r="AO37" s="39"/>
       <c r="AP37" s="39">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AQ37" s="39"/>
       <c r="AR37" s="39"/>
       <c r="AS37" s="39">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AT37" s="39"/>
       <c r="AU37" s="39"/>
       <c r="AV37" s="39">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW37" s="39"/>
       <c r="AX37" s="39"/>
       <c r="AY37" s="39">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AZ37" s="35">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="BA37" s="35">
         <f>G37-AZ37</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="BB37" s="2"/>
     </row>
-    <row r="38" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:54" s="41" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="42"/>
       <c r="C38" s="37"/>
       <c r="D38" s="36" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="E38" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="F38" s="39" t="s">
-        <v>68</v>
+      <c r="F38" s="42" t="s">
+        <v>62</v>
       </c>
       <c r="G38" s="43">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H38" s="39"/>
       <c r="I38" s="39">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J38" s="39"/>
       <c r="K38" s="39"/>
       <c r="L38" s="39">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M38" s="39"/>
       <c r="N38" s="39"/>
       <c r="O38" s="39">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P38" s="39"/>
       <c r="Q38" s="39"/>
       <c r="R38" s="39">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S38" s="39"/>
       <c r="T38" s="39"/>
       <c r="U38" s="39">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V38" s="39"/>
       <c r="W38" s="39"/>
       <c r="X38" s="39">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y38" s="39"/>
-      <c r="Z38" s="39"/>
+      <c r="Z38" s="39">
+        <v>1</v>
+      </c>
       <c r="AA38" s="39">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AB38" s="39"/>
       <c r="AC38" s="39"/>
       <c r="AD38" s="39">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AE38" s="39"/>
       <c r="AF38" s="39"/>
       <c r="AG38" s="39">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH38" s="39"/>
       <c r="AI38" s="39"/>
       <c r="AJ38" s="39">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AK38" s="39"/>
       <c r="AL38" s="39">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AM38" s="39">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="AN38" s="39"/>
       <c r="AO38" s="39"/>
       <c r="AP38" s="39">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="AQ38" s="39"/>
       <c r="AR38" s="39"/>
       <c r="AS38" s="39">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="AT38" s="39"/>
       <c r="AU38" s="39"/>
       <c r="AV38" s="39">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="AW38" s="39"/>
       <c r="AX38" s="39"/>
       <c r="AY38" s="39">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="AZ38" s="35">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="BA38" s="35">
         <f>G38-AZ38</f>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="BB38" s="2"/>
     </row>
-    <row r="39" spans="2:54" s="41" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="43"/>
+    <row r="39" spans="2:54" s="41" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="42"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F39" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G39" s="43">
+        <v>2</v>
+      </c>
       <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
+      <c r="I39" s="39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="J39" s="39"/>
       <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
+      <c r="L39" s="39">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
       <c r="M39" s="39"/>
       <c r="N39" s="39"/>
-      <c r="O39" s="39"/>
+      <c r="O39" s="39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="P39" s="39"/>
       <c r="Q39" s="39"/>
-      <c r="R39" s="39"/>
+      <c r="R39" s="39">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
       <c r="S39" s="39"/>
       <c r="T39" s="39"/>
-      <c r="U39" s="39"/>
+      <c r="U39" s="39">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
       <c r="V39" s="39"/>
       <c r="W39" s="39"/>
-      <c r="X39" s="39"/>
+      <c r="X39" s="39">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
       <c r="Y39" s="39"/>
-      <c r="Z39" s="39"/>
-      <c r="AA39" s="39"/>
+      <c r="Z39" s="39">
+        <v>2</v>
+      </c>
+      <c r="AA39" s="39">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AB39" s="39"/>
       <c r="AC39" s="39"/>
-      <c r="AD39" s="39"/>
+      <c r="AD39" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="AE39" s="39"/>
       <c r="AF39" s="39"/>
-      <c r="AG39" s="39"/>
+      <c r="AG39" s="39">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="AH39" s="39"/>
       <c r="AI39" s="39"/>
-      <c r="AJ39" s="39"/>
+      <c r="AJ39" s="39">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="AK39" s="39"/>
       <c r="AL39" s="39"/>
-      <c r="AM39" s="39"/>
+      <c r="AM39" s="39">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="AN39" s="39"/>
       <c r="AO39" s="39"/>
-      <c r="AP39" s="39"/>
+      <c r="AP39" s="39">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AQ39" s="39"/>
       <c r="AR39" s="39"/>
-      <c r="AS39" s="39"/>
+      <c r="AS39" s="39">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
       <c r="AT39" s="39"/>
       <c r="AU39" s="39"/>
-      <c r="AV39" s="39"/>
+      <c r="AV39" s="39">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
       <c r="AW39" s="39"/>
       <c r="AX39" s="39"/>
-      <c r="AY39" s="39"/>
-      <c r="AZ39" s="35"/>
-      <c r="BA39" s="35"/>
+      <c r="AY39" s="39">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AZ39" s="35">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="BA39" s="35">
+        <f>G39-AZ39</f>
+        <v>0</v>
+      </c>
       <c r="BB39" s="2"/>
     </row>
-    <row r="40" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="42"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="E40" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="F40" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="G40" s="43">
-        <v>2</v>
-      </c>
+    <row r="40" spans="2:54" s="41" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="40"/>
       <c r="H40" s="39"/>
-      <c r="I40" s="39">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
+      <c r="I40" s="39"/>
       <c r="J40" s="39"/>
       <c r="K40" s="39"/>
-      <c r="L40" s="39">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
+      <c r="L40" s="39"/>
       <c r="M40" s="39"/>
       <c r="N40" s="39"/>
-      <c r="O40" s="39">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
+      <c r="O40" s="39"/>
       <c r="P40" s="39"/>
-      <c r="Q40" s="39">
-        <v>2</v>
-      </c>
-      <c r="R40" s="39">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="Q40" s="39"/>
+      <c r="R40" s="39"/>
       <c r="S40" s="39"/>
       <c r="T40" s="39"/>
-      <c r="U40" s="39">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+      <c r="U40" s="39"/>
       <c r="V40" s="39"/>
       <c r="W40" s="39"/>
-      <c r="X40" s="39">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="X40" s="39"/>
       <c r="Y40" s="39"/>
       <c r="Z40" s="39"/>
-      <c r="AA40" s="39">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
+      <c r="AA40" s="39"/>
       <c r="AB40" s="39"/>
       <c r="AC40" s="39"/>
-      <c r="AD40" s="39">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="AD40" s="39"/>
       <c r="AE40" s="39"/>
       <c r="AF40" s="39"/>
-      <c r="AG40" s="39">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
+      <c r="AG40" s="39"/>
       <c r="AH40" s="39"/>
       <c r="AI40" s="39"/>
-      <c r="AJ40" s="39">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
+      <c r="AJ40" s="39"/>
       <c r="AK40" s="39"/>
       <c r="AL40" s="39"/>
-      <c r="AM40" s="39">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+      <c r="AM40" s="39"/>
       <c r="AN40" s="39"/>
       <c r="AO40" s="39"/>
-      <c r="AP40" s="39">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
+      <c r="AP40" s="39"/>
       <c r="AQ40" s="39"/>
       <c r="AR40" s="39"/>
-      <c r="AS40" s="39">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
+      <c r="AS40" s="39"/>
       <c r="AT40" s="39"/>
       <c r="AU40" s="39"/>
-      <c r="AV40" s="39">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
+      <c r="AV40" s="39"/>
       <c r="AW40" s="39"/>
       <c r="AX40" s="39"/>
-      <c r="AY40" s="39">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AZ40" s="35">
-        <f t="shared" si="14"/>
-        <v>2</v>
-      </c>
-      <c r="BA40" s="35">
-        <f t="shared" ref="BA40:BA42" si="17">G40-AZ40</f>
-        <v>0</v>
-      </c>
+      <c r="AY40" s="39"/>
+      <c r="AZ40" s="35"/>
+      <c r="BA40" s="35"/>
       <c r="BB40" s="2"/>
     </row>
-    <row r="41" spans="2:54" s="41" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="43"/>
+    <row r="41" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="42"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="G41" s="43">
+        <v>2</v>
+      </c>
       <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
+      <c r="I41" s="39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="J41" s="39"/>
       <c r="K41" s="39"/>
-      <c r="L41" s="39"/>
+      <c r="L41" s="39">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
       <c r="M41" s="39"/>
       <c r="N41" s="39"/>
-      <c r="O41" s="39"/>
+      <c r="O41" s="39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="P41" s="39"/>
       <c r="Q41" s="39"/>
-      <c r="R41" s="39"/>
+      <c r="R41" s="39">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
       <c r="S41" s="39"/>
       <c r="T41" s="39"/>
-      <c r="U41" s="39"/>
+      <c r="U41" s="39">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
       <c r="V41" s="39"/>
-      <c r="W41" s="39"/>
-      <c r="X41" s="39"/>
+      <c r="W41" s="39">
+        <v>1</v>
+      </c>
+      <c r="X41" s="39">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
       <c r="Y41" s="39"/>
       <c r="Z41" s="39"/>
-      <c r="AA41" s="39"/>
+      <c r="AA41" s="39">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
       <c r="AB41" s="39"/>
       <c r="AC41" s="39"/>
-      <c r="AD41" s="39"/>
+      <c r="AD41" s="39">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
       <c r="AE41" s="39"/>
       <c r="AF41" s="39"/>
-      <c r="AG41" s="39"/>
+      <c r="AG41" s="39">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="AH41" s="39"/>
       <c r="AI41" s="39"/>
-      <c r="AJ41" s="39"/>
+      <c r="AJ41" s="39">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
       <c r="AK41" s="39"/>
-      <c r="AL41" s="39"/>
-      <c r="AM41" s="39"/>
+      <c r="AL41" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="AM41" s="39">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
       <c r="AN41" s="39"/>
       <c r="AO41" s="39"/>
-      <c r="AP41" s="39"/>
+      <c r="AP41" s="39">
+        <f t="shared" si="11"/>
+        <v>0.5</v>
+      </c>
       <c r="AQ41" s="39"/>
       <c r="AR41" s="39"/>
-      <c r="AS41" s="39"/>
+      <c r="AS41" s="39">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
       <c r="AT41" s="39"/>
       <c r="AU41" s="39"/>
-      <c r="AV41" s="39"/>
+      <c r="AV41" s="39">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
       <c r="AW41" s="39"/>
       <c r="AX41" s="39"/>
-      <c r="AY41" s="39"/>
-      <c r="AZ41" s="35"/>
-      <c r="BA41" s="35"/>
+      <c r="AY41" s="39">
+        <f t="shared" si="15"/>
+        <v>0.5</v>
+      </c>
+      <c r="AZ41" s="35">
+        <f t="shared" si="14"/>
+        <v>1.5</v>
+      </c>
+      <c r="BA41" s="35">
+        <f>G41-AZ41</f>
+        <v>0.5</v>
+      </c>
       <c r="BB41" s="2"/>
     </row>
     <row r="42" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="42"/>
       <c r="C42" s="37"/>
       <c r="D42" s="36" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E42" s="36" t="s">
         <v>42</v>
@@ -4764,15 +4792,15 @@
         <v>2</v>
       </c>
       <c r="S42" s="39"/>
-      <c r="T42" s="39">
-        <v>1</v>
-      </c>
+      <c r="T42" s="39"/>
       <c r="U42" s="39">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V42" s="39"/>
-      <c r="W42" s="39"/>
+      <c r="W42" s="39">
+        <v>1</v>
+      </c>
       <c r="X42" s="39">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -4802,106 +4830,685 @@
         <v>1</v>
       </c>
       <c r="AK42" s="39"/>
-      <c r="AL42" s="39"/>
+      <c r="AL42" s="39">
+        <v>0.5</v>
+      </c>
       <c r="AM42" s="39">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AN42" s="39"/>
       <c r="AO42" s="39"/>
       <c r="AP42" s="39">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AQ42" s="39"/>
       <c r="AR42" s="39"/>
       <c r="AS42" s="39">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AT42" s="39"/>
       <c r="AU42" s="39"/>
       <c r="AV42" s="39">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW42" s="39"/>
       <c r="AX42" s="39"/>
       <c r="AY42" s="39">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AZ42" s="35">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="BA42" s="35">
-        <f t="shared" si="17"/>
-        <v>1</v>
+        <f>G42-AZ42</f>
+        <v>0.5</v>
       </c>
       <c r="BB42" s="2"/>
     </row>
-    <row r="43" spans="2:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="45"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="14"/>
-      <c r="U43" s="14"/>
-      <c r="V43" s="15"/>
-      <c r="W43" s="14"/>
-      <c r="X43" s="14"/>
-      <c r="Y43" s="15"/>
-      <c r="Z43" s="14"/>
-      <c r="AA43" s="14"/>
-      <c r="AB43" s="15"/>
-      <c r="AC43" s="14"/>
-      <c r="AD43" s="14"/>
-      <c r="AE43" s="15"/>
-      <c r="AF43" s="14"/>
-      <c r="AG43" s="14"/>
-      <c r="AH43" s="15"/>
-      <c r="AI43" s="14"/>
-      <c r="AJ43" s="14"/>
-      <c r="AK43" s="15"/>
-      <c r="AL43" s="14"/>
-      <c r="AM43" s="14"/>
-      <c r="AN43" s="15"/>
-      <c r="AO43" s="14"/>
-      <c r="AP43" s="14"/>
-      <c r="AQ43" s="15"/>
-      <c r="AR43" s="14"/>
-      <c r="AS43" s="14"/>
-      <c r="AT43" s="15"/>
-      <c r="AU43" s="14"/>
-      <c r="AV43" s="14"/>
-      <c r="AW43" s="15"/>
-      <c r="AX43" s="14"/>
-      <c r="AY43" s="14"/>
-      <c r="AZ43" s="14"/>
-      <c r="BA43" s="14"/>
+    <row r="43" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="42"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F43" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="G43" s="43">
+        <v>2</v>
+      </c>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J43" s="39"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="39">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M43" s="39"/>
+      <c r="N43" s="39"/>
+      <c r="O43" s="39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P43" s="39"/>
+      <c r="Q43" s="39"/>
+      <c r="R43" s="39">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="S43" s="39"/>
+      <c r="T43" s="39"/>
+      <c r="U43" s="39">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="V43" s="39"/>
+      <c r="W43" s="39"/>
+      <c r="X43" s="39">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Y43" s="39"/>
+      <c r="Z43" s="39"/>
+      <c r="AA43" s="39">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="AB43" s="39"/>
+      <c r="AC43" s="39">
+        <v>1</v>
+      </c>
+      <c r="AD43" s="39">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="AE43" s="39"/>
+      <c r="AF43" s="39"/>
+      <c r="AG43" s="39">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AH43" s="39"/>
+      <c r="AI43" s="39"/>
+      <c r="AJ43" s="39">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="AK43" s="39"/>
+      <c r="AL43" s="39"/>
+      <c r="AM43" s="39">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AN43" s="39"/>
+      <c r="AO43" s="39"/>
+      <c r="AP43" s="39">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AQ43" s="39"/>
+      <c r="AR43" s="39"/>
+      <c r="AS43" s="39">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AT43" s="39"/>
+      <c r="AU43" s="39"/>
+      <c r="AV43" s="39">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AW43" s="39"/>
+      <c r="AX43" s="39"/>
+      <c r="AY43" s="39">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="AZ43" s="35">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="BA43" s="35">
+        <f>G43-AZ43</f>
+        <v>1</v>
+      </c>
+      <c r="BB43" s="2"/>
+    </row>
+    <row r="44" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="42"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="G44" s="43">
+        <v>4</v>
+      </c>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J44" s="39"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="39">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M44" s="39"/>
+      <c r="N44" s="39"/>
+      <c r="O44" s="39">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="P44" s="39"/>
+      <c r="Q44" s="39"/>
+      <c r="R44" s="39">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="S44" s="39"/>
+      <c r="T44" s="39"/>
+      <c r="U44" s="39">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="V44" s="39"/>
+      <c r="W44" s="39"/>
+      <c r="X44" s="39">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="Y44" s="39"/>
+      <c r="Z44" s="39"/>
+      <c r="AA44" s="39">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AB44" s="39"/>
+      <c r="AC44" s="39"/>
+      <c r="AD44" s="39">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="AE44" s="39"/>
+      <c r="AF44" s="39"/>
+      <c r="AG44" s="39">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AH44" s="39"/>
+      <c r="AI44" s="39"/>
+      <c r="AJ44" s="39">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="AK44" s="39"/>
+      <c r="AL44" s="39">
+        <v>1</v>
+      </c>
+      <c r="AM44" s="39">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="AN44" s="39"/>
+      <c r="AO44" s="39"/>
+      <c r="AP44" s="39">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="AQ44" s="39"/>
+      <c r="AR44" s="39"/>
+      <c r="AS44" s="39">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="AT44" s="39"/>
+      <c r="AU44" s="39"/>
+      <c r="AV44" s="39">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="AW44" s="39"/>
+      <c r="AX44" s="39"/>
+      <c r="AY44" s="39">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="AZ44" s="35">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="BA44" s="35">
+        <f>G44-AZ44</f>
+        <v>3</v>
+      </c>
+      <c r="BB44" s="2"/>
+    </row>
+    <row r="45" spans="2:54" s="41" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="39"/>
+      <c r="L45" s="39"/>
+      <c r="M45" s="39"/>
+      <c r="N45" s="39"/>
+      <c r="O45" s="39"/>
+      <c r="P45" s="39"/>
+      <c r="Q45" s="39"/>
+      <c r="R45" s="39"/>
+      <c r="S45" s="39"/>
+      <c r="T45" s="39"/>
+      <c r="U45" s="39"/>
+      <c r="V45" s="39"/>
+      <c r="W45" s="39"/>
+      <c r="X45" s="39"/>
+      <c r="Y45" s="39"/>
+      <c r="Z45" s="39"/>
+      <c r="AA45" s="39"/>
+      <c r="AB45" s="39"/>
+      <c r="AC45" s="39"/>
+      <c r="AD45" s="39"/>
+      <c r="AE45" s="39"/>
+      <c r="AF45" s="39"/>
+      <c r="AG45" s="39"/>
+      <c r="AH45" s="39"/>
+      <c r="AI45" s="39"/>
+      <c r="AJ45" s="39"/>
+      <c r="AK45" s="39"/>
+      <c r="AL45" s="39"/>
+      <c r="AM45" s="39"/>
+      <c r="AN45" s="39"/>
+      <c r="AO45" s="39"/>
+      <c r="AP45" s="39"/>
+      <c r="AQ45" s="39"/>
+      <c r="AR45" s="39"/>
+      <c r="AS45" s="39"/>
+      <c r="AT45" s="39"/>
+      <c r="AU45" s="39"/>
+      <c r="AV45" s="39"/>
+      <c r="AW45" s="39"/>
+      <c r="AX45" s="39"/>
+      <c r="AY45" s="39"/>
+      <c r="AZ45" s="35"/>
+      <c r="BA45" s="35"/>
+      <c r="BB45" s="2"/>
+    </row>
+    <row r="46" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="42"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F46" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="G46" s="43">
+        <v>2</v>
+      </c>
+      <c r="H46" s="39"/>
+      <c r="I46" s="39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J46" s="39"/>
+      <c r="K46" s="39"/>
+      <c r="L46" s="39">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M46" s="39"/>
+      <c r="N46" s="39"/>
+      <c r="O46" s="39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P46" s="39"/>
+      <c r="Q46" s="39">
+        <v>2</v>
+      </c>
+      <c r="R46" s="39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S46" s="39"/>
+      <c r="T46" s="39"/>
+      <c r="U46" s="39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V46" s="39"/>
+      <c r="W46" s="39"/>
+      <c r="X46" s="39">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Y46" s="39"/>
+      <c r="Z46" s="39"/>
+      <c r="AA46" s="39">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AB46" s="39"/>
+      <c r="AC46" s="39"/>
+      <c r="AD46" s="39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AE46" s="39"/>
+      <c r="AF46" s="39"/>
+      <c r="AG46" s="39">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AH46" s="39"/>
+      <c r="AI46" s="39"/>
+      <c r="AJ46" s="39">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AK46" s="39"/>
+      <c r="AL46" s="39"/>
+      <c r="AM46" s="39">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AN46" s="39"/>
+      <c r="AO46" s="39"/>
+      <c r="AP46" s="39">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AQ46" s="39"/>
+      <c r="AR46" s="39"/>
+      <c r="AS46" s="39">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AT46" s="39"/>
+      <c r="AU46" s="39"/>
+      <c r="AV46" s="39">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AW46" s="39"/>
+      <c r="AX46" s="39"/>
+      <c r="AY46" s="39">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AZ46" s="35">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="BA46" s="35">
+        <f t="shared" ref="BA46:BA48" si="44">G46-AZ46</f>
+        <v>0</v>
+      </c>
+      <c r="BB46" s="2"/>
+    </row>
+    <row r="47" spans="2:54" s="41" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="39"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
+      <c r="K47" s="39"/>
+      <c r="L47" s="39"/>
+      <c r="M47" s="39"/>
+      <c r="N47" s="39"/>
+      <c r="O47" s="39"/>
+      <c r="P47" s="39"/>
+      <c r="Q47" s="39"/>
+      <c r="R47" s="39"/>
+      <c r="S47" s="39"/>
+      <c r="T47" s="39"/>
+      <c r="U47" s="39"/>
+      <c r="V47" s="39"/>
+      <c r="W47" s="39"/>
+      <c r="X47" s="39"/>
+      <c r="Y47" s="39"/>
+      <c r="Z47" s="39"/>
+      <c r="AA47" s="39"/>
+      <c r="AB47" s="39"/>
+      <c r="AC47" s="39"/>
+      <c r="AD47" s="39"/>
+      <c r="AE47" s="39"/>
+      <c r="AF47" s="39"/>
+      <c r="AG47" s="39"/>
+      <c r="AH47" s="39"/>
+      <c r="AI47" s="39"/>
+      <c r="AJ47" s="39"/>
+      <c r="AK47" s="39"/>
+      <c r="AL47" s="39"/>
+      <c r="AM47" s="39"/>
+      <c r="AN47" s="39"/>
+      <c r="AO47" s="39"/>
+      <c r="AP47" s="39"/>
+      <c r="AQ47" s="39"/>
+      <c r="AR47" s="39"/>
+      <c r="AS47" s="39"/>
+      <c r="AT47" s="39"/>
+      <c r="AU47" s="39"/>
+      <c r="AV47" s="39"/>
+      <c r="AW47" s="39"/>
+      <c r="AX47" s="39"/>
+      <c r="AY47" s="39"/>
+      <c r="AZ47" s="35"/>
+      <c r="BA47" s="35"/>
+      <c r="BB47" s="2"/>
+    </row>
+    <row r="48" spans="2:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="42"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="G48" s="43">
+        <v>2</v>
+      </c>
+      <c r="H48" s="39"/>
+      <c r="I48" s="39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J48" s="39"/>
+      <c r="K48" s="39"/>
+      <c r="L48" s="39">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M48" s="39"/>
+      <c r="N48" s="39"/>
+      <c r="O48" s="39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P48" s="39"/>
+      <c r="Q48" s="39"/>
+      <c r="R48" s="39">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="S48" s="39"/>
+      <c r="T48" s="39">
+        <v>1</v>
+      </c>
+      <c r="U48" s="39">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="V48" s="39"/>
+      <c r="W48" s="39"/>
+      <c r="X48" s="39">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Y48" s="39"/>
+      <c r="Z48" s="39"/>
+      <c r="AA48" s="39">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AB48" s="39"/>
+      <c r="AC48" s="39"/>
+      <c r="AD48" s="39">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="AE48" s="39"/>
+      <c r="AF48" s="39"/>
+      <c r="AG48" s="39">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AH48" s="39"/>
+      <c r="AI48" s="39"/>
+      <c r="AJ48" s="39">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="AK48" s="39"/>
+      <c r="AL48" s="39"/>
+      <c r="AM48" s="39">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AN48" s="39"/>
+      <c r="AO48" s="39"/>
+      <c r="AP48" s="39">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AQ48" s="39"/>
+      <c r="AR48" s="39"/>
+      <c r="AS48" s="39">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AT48" s="39"/>
+      <c r="AU48" s="39"/>
+      <c r="AV48" s="39">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AW48" s="39"/>
+      <c r="AX48" s="39"/>
+      <c r="AY48" s="39">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="AZ48" s="35">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="BA48" s="35">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="BB48" s="2"/>
+    </row>
+    <row r="49" spans="2:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="45"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="14"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="14"/>
+      <c r="R49" s="14"/>
+      <c r="S49" s="15"/>
+      <c r="T49" s="14"/>
+      <c r="U49" s="14"/>
+      <c r="V49" s="15"/>
+      <c r="W49" s="14"/>
+      <c r="X49" s="14"/>
+      <c r="Y49" s="15"/>
+      <c r="Z49" s="14"/>
+      <c r="AA49" s="14"/>
+      <c r="AB49" s="15"/>
+      <c r="AC49" s="14"/>
+      <c r="AD49" s="14"/>
+      <c r="AE49" s="15"/>
+      <c r="AF49" s="14"/>
+      <c r="AG49" s="14"/>
+      <c r="AH49" s="15"/>
+      <c r="AI49" s="14"/>
+      <c r="AJ49" s="14"/>
+      <c r="AK49" s="15"/>
+      <c r="AL49" s="14"/>
+      <c r="AM49" s="14"/>
+      <c r="AN49" s="15"/>
+      <c r="AO49" s="14"/>
+      <c r="AP49" s="14"/>
+      <c r="AQ49" s="15"/>
+      <c r="AR49" s="14"/>
+      <c r="AS49" s="14"/>
+      <c r="AT49" s="15"/>
+      <c r="AU49" s="14"/>
+      <c r="AV49" s="14"/>
+      <c r="AW49" s="15"/>
+      <c r="AX49" s="14"/>
+      <c r="AY49" s="14"/>
+      <c r="AZ49" s="14"/>
+      <c r="BA49" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -4913,6 +5520,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>